<commit_message>
added load_workbook and started model
</commit_message>
<xml_diff>
--- a/test_case_workbook.v2.xlsx
+++ b/test_case_workbook.v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1020" windowWidth="23960" windowHeight="15120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2300" yWindow="2260" windowWidth="23960" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="182">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>This test case runs the process with a good dataset and expects all data to be processed and loaded successfully</t>
-  </si>
-  <si>
-    <t>David Moore</t>
   </si>
   <si>
     <t>Process with bad data, expecting data to be rejected</t>
@@ -686,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -727,9 +724,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1032,11 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1045,32 +1039,24 @@
     <col min="2" max="2" width="9.5" style="15" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="35.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1083,14 +1069,8 @@
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="17">
-        <v>42552</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1098,153 +1078,113 @@
         <v>6</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="17">
-        <v>42552</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1261,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
@@ -1284,48 +1224,48 @@
     <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:14" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="L1" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="L1" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>158</v>
+      <c r="N1" s="18" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -1339,34 +1279,34 @@
         <v>6</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="G2" s="14" t="str">
         <f>IF(F2="","",IF(ISNA(VLOOKUP($F2&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F2&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Sheet Name</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="14" t="str">
         <f>IF(H2="","",IF(ISNA(VLOOKUP($F2&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F2&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>File Path Name</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K2" s="14" t="str">
         <f>IF(J2="","",IF(ISNA(VLOOKUP($F2&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F2&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>File Format</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" s="14" t="str">
         <f>IF(L2="","",IF(ISNA(VLOOKUP($F2&amp;"-"&amp;MID($M$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F2&amp;"-"&amp;MID($M$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1385,27 +1325,27 @@
         <v>6</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="G3" s="14" t="str">
         <f>IF(F3="","",IF(ISNA(VLOOKUP($F3&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F3&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>SQL</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3" s="14" t="str">
         <f>IF(H3="","",IF(ISNA(VLOOKUP($F3&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F3&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Connection</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="14" t="str">
         <f>IF(J3="","",IF(ISNA(VLOOKUP($F3&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F3&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1429,20 +1369,20 @@
         <v>6</v>
       </c>
       <c r="D4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="14" t="str">
         <f>IF(F4="","",IF(ISNA(VLOOKUP($F4&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F4&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Command</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I4" s="14" t="str">
         <f>IF(H4="","",IF(ISNA(VLOOKUP($F4&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F4&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1471,20 +1411,20 @@
         <v>6</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" s="14" t="str">
         <f>IF(F5="","",IF(ISNA(VLOOKUP($F5&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F5&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Expected Return Code</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I5" s="14" t="str">
         <f>IF(H5="","",IF(ISNA(VLOOKUP($F5&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F5&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1513,27 +1453,27 @@
         <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="G6" s="14" t="str">
         <f>IF(F6="","",IF(ISNA(VLOOKUP($F6&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F6&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>SQL</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="14" t="str">
         <f>IF(H6="","",IF(ISNA(VLOOKUP($F6&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F6&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Connection</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="14" t="str">
         <f>IF(J6="","",IF(ISNA(VLOOKUP($F6&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F6&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1557,34 +1497,34 @@
         <v>6</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="14" t="str">
         <f>IF(F7="","",IF(ISNA(VLOOKUP($F7&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F7&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Sheet Name</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I7" s="14" t="str">
         <f>IF(H7="","",IF(ISNA(VLOOKUP($F7&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F7&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Table Name</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K7" s="14" t="str">
         <f>IF(J7="","",IF(ISNA(VLOOKUP($F7&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F7&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Connection</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="14" t="str">
         <f>IF(L7="","",IF(ISNA(VLOOKUP($F7&amp;"-"&amp;MID($M$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F7&amp;"-"&amp;MID($M$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1603,34 +1543,34 @@
         <v>6</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="G8" s="14" t="str">
         <f>IF(F8="","",IF(ISNA(VLOOKUP($F8&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F8&amp;"-"&amp;MID($G$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Expected Dataset</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="14" t="str">
         <f>IF(H8="","",IF(ISNA(VLOOKUP($F8&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F8&amp;"-"&amp;MID($I$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Expected Dataset Type</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K8" s="14" t="str">
         <f>IF(J8="","",IF(ISNA(VLOOKUP($F8&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F8&amp;"-"&amp;MID($K$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
         <v>Actual Dataset</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M8" s="14" t="str">
         <f>IF(L8="","",IF(ISNA(VLOOKUP($F8&amp;"-"&amp;MID($M$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)),"",VLOOKUP($F8&amp;"-"&amp;MID($M$1,11,1),'Command Parameters'!$C$2:$D$27,2,FALSE)))</f>
@@ -1737,18 +1677,18 @@
     <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:4" s="20" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>45</v>
+      <c r="D1" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1756,13 +1696,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1770,25 +1710,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1796,13 +1736,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1810,13 +1750,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1824,10 +1764,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="8"/>
     </row>
@@ -1836,10 +1776,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="D8" s="8"/>
     </row>
@@ -1848,10 +1788,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="8"/>
     </row>
@@ -2071,47 +2011,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>45</v>
+      <c r="C1" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2316,19 +2256,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2336,10 +2276,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="D2" s="11">
         <v>113999</v>
@@ -2353,10 +2293,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="D3" s="11">
         <v>40951</v>
@@ -2415,19 +2355,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2435,10 +2375,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" s="11">
         <v>39612</v>
@@ -2452,10 +2392,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="D3" s="11">
         <v>38818</v>
@@ -2469,10 +2409,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="D4" s="11">
         <v>34556</v>
@@ -2486,10 +2426,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" s="11">
         <v>37339</v>
@@ -2503,10 +2443,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>142</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>143</v>
       </c>
       <c r="D6" s="11">
         <v>41262</v>
@@ -2520,10 +2460,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="D7" s="11">
         <v>38818</v>
@@ -2555,107 +2495,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>45</v>
+      <c r="A1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2683,25 +2623,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="24" t="s">
+      <c r="A1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2711,15 +2651,15 @@
         <v>Execute SQL-1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2729,15 +2669,15 @@
         <v>Execute SQL-2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -2747,15 +2687,15 @@
         <v>Execute SQL With Result-1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2765,15 +2705,15 @@
         <v>Execute SQL With Result-2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2783,15 +2723,15 @@
         <v>Execute SQL With Result To Parameter-1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -2801,15 +2741,15 @@
         <v>Execute SQL With Result To Parameter-2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -2819,15 +2759,15 @@
         <v>Execute SQL With Result To Parameter-3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -2837,15 +2777,15 @@
         <v>Execute Shell Command-1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2855,15 +2795,15 @@
         <v>Load Sheet to Table-1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -2873,15 +2813,15 @@
         <v>Load Sheet to Table-2</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
@@ -2891,15 +2831,15 @@
         <v>Load Sheet to Table-3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -2909,15 +2849,15 @@
         <v>Save Sheet to File-1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -2927,15 +2867,15 @@
         <v>Save Sheet to File-2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -2945,15 +2885,15 @@
         <v>Save Sheet to File-3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -2963,15 +2903,15 @@
         <v>Assert Datasets Equal-1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -2981,15 +2921,15 @@
         <v>Assert Datasets Equal-2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
@@ -2999,15 +2939,15 @@
         <v>Assert Datasets Equal-3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
@@ -3017,15 +2957,15 @@
         <v>Assert Datasets Equal-4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -3035,15 +2975,15 @@
         <v>Assert SQL Records Returned-1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -3053,15 +2993,15 @@
         <v>Assert SQL Records Returned-2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -3071,15 +3011,15 @@
         <v>Assert SQL No Records Returned-1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
@@ -3089,15 +3029,15 @@
         <v>Assert SQL No Records Returned-2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -3107,15 +3047,15 @@
         <v>Assert SQL Single Value Returned-1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -3125,15 +3065,15 @@
         <v>Assert SQL Single Value Returned-2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -3143,15 +3083,15 @@
         <v>Assert Last Return Code Equal-1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -3161,10 +3101,10 @@
         <v>Assert Last Return Code Not Equal-1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3196,281 +3136,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>45</v>
+      <c r="A1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>